<commit_message>
Created multi-modal communication observation and added the appropriate code systems and value sets
</commit_message>
<xml_diff>
--- a/output/CodeSystem-SPLASCHObservationCategoryCS.xlsx
+++ b/output/CodeSystem-SPLASCHObservationCategoryCS.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-12-29T13:00:19-05:00</t>
+    <t>2022-03-14T15:55:03-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -123,7 +123,7 @@
     <t>Count</t>
   </si>
   <si>
-    <t>3</t>
+    <t>5</t>
   </si>
   <si>
     <t>Level</t>
@@ -166,6 +166,24 @@
   </si>
   <si>
     <t>Category code for swallowing observation</t>
+  </si>
+  <si>
+    <t>multi-modal-communication</t>
+  </si>
+  <si>
+    <t>Multi-modal communication</t>
+  </si>
+  <si>
+    <t>Category code for multi-modal communication observation</t>
+  </si>
+  <si>
+    <t>hearing</t>
+  </si>
+  <si>
+    <t>Hearing</t>
+  </si>
+  <si>
+    <t>Category code for hearing observation</t>
   </si>
 </sst>
 </file>
@@ -486,7 +504,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -548,6 +566,34 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>